<commit_message>
Carga masiva de productos
</commit_message>
<xml_diff>
--- a/public/uploads/formats/products_charge.xlsx
+++ b/public/uploads/formats/products_charge.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marzioperez/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac Abensur\Documents\Proyectos\backend-regalalo\public\uploads\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912747F0-AF80-4948-99BA-C5C16CB67F14}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="27200" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="38400" yWindow="465" windowWidth="27195" windowHeight="14895" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,100 +28,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
-  <si>
-    <t>Razón social</t>
-  </si>
-  <si>
-    <t>RUC</t>
-  </si>
-  <si>
-    <t>Dirección Legal</t>
-  </si>
-  <si>
-    <t>Teléfono</t>
-  </si>
-  <si>
-    <t>Nombre Comercial</t>
-  </si>
-  <si>
-    <t>Nombres y Apellidos</t>
-  </si>
-  <si>
-    <t>Legal</t>
-  </si>
-  <si>
-    <t>DNI / CE</t>
-  </si>
-  <si>
-    <t>Representante Legal</t>
-  </si>
-  <si>
-    <t>Comercial</t>
-  </si>
-  <si>
-    <t>Contacto Comercial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNI / CE </t>
-  </si>
-  <si>
-    <t>Teléfono / Celular</t>
-  </si>
-  <si>
-    <t>Correo electrónico</t>
-  </si>
-  <si>
-    <t>Entidad Financiera</t>
-  </si>
-  <si>
-    <t>Tipo de Cuenta</t>
-  </si>
-  <si>
-    <t>Nombre del Estado de Cuenta</t>
-  </si>
-  <si>
-    <t>Numero de Cuenta Bancaria</t>
-  </si>
-  <si>
-    <t>Código CCI</t>
-  </si>
-  <si>
-    <t>Financiero</t>
-  </si>
-  <si>
-    <t>PayMe</t>
-  </si>
-  <si>
-    <t>Analytics</t>
-  </si>
-  <si>
-    <t>ID Comercio</t>
-  </si>
-  <si>
-    <t>ID Wallet</t>
-  </si>
-  <si>
-    <t>ID GA</t>
-  </si>
-  <si>
-    <t>URL de la Tienda</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Nombre del producto</t>
+  </si>
+  <si>
+    <t>Codigo SKU</t>
+  </si>
+  <si>
+    <t>Descuento</t>
+  </si>
+  <si>
+    <t>Presentación del producto</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Edades</t>
+  </si>
+  <si>
+    <t>Envío</t>
+  </si>
+  <si>
+    <t>Precio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -148,12 +87,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -163,6 +98,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -430,139 +368,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" customWidth="1"/>
+    <col min="5" max="5" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.375" customWidth="1"/>
+    <col min="7" max="7" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.375" customWidth="1"/>
+    <col min="10" max="10" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="S1" s="1"/>
-      <c r="T1" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>18</v>
-      </c>
-      <c r="R2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S2" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="M1:Q1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cargas masivas, características de producto, fix varios
</commit_message>
<xml_diff>
--- a/public/uploads/formats/products_charge.xlsx
+++ b/public/uploads/formats/products_charge.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac Abensur\Documents\Proyectos\backend-regalalo\public\uploads\formats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Propietario\Documents\Proyectos\backend-regalalo\public\uploads\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912747F0-AF80-4948-99BA-C5C16CB67F14}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="465" windowWidth="27195" windowHeight="14895" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="465" windowWidth="27195" windowHeight="14895" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,6 +23,243 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Isaac Abensur</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>regalalo.pe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+El nombre del producto es obligatorio. Sino se consigna no se registrará en la plataforma.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Regalalo.pe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+El código SKU es único. Si existe entre los productos que haya creado hasta el momento, los datos se actualizarán, en su defecto, se creará un  nuevo registro.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>regalalo.pe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+El descuento se consigna del 0 al 99 en la parte entera y como máximo dos digitos en la parte decimal.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Regalalo.pe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+El precio solo acepta números sin símbolos de moneda, sin separación de miles o millares y como máximo dos digitos en la parte decimal.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>regalalo.pe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+La presentación del producto, solo acepta lo siguientes valores, sin espacios y todo en minúsculas:
+- unidad
+- par
+- caja
+- docena</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>regalalo.pe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+La descripción acepta todo tipo de texto.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>regalalo.pe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+El rango de edades a los cuales está dirigido el producto se consigna como sigue:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>edad_mínima,edad_maxima</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Donde:
+edad_mínima: Solo puede ser un valor entero y debe ser menor a la edad máxima
+edad_maxima: Solo puede ser un valor entero y debe ser mayor a la edad mínima</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>regalalo.pe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+El envío solo acepta los siguientes valores en mayúsculas y sin espacios:
+- D
+- S
+- A
+Donde:
+D: Solo Delivery
+S: Recojo en Tienda
+A: Ambos (Delivery y Recojo en tienda)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
@@ -57,14 +290,34 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -368,11 +621,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -423,5 +676,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>